<commit_message>
Added aditional formatting and highlighted some of the most likely candidates for marionette usage
</commit_message>
<xml_diff>
--- a/STM32matrix.xlsx
+++ b/STM32matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="500" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="1020" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -503,12 +503,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -567,11 +573,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -579,6 +582,17 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -627,97 +641,7 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1078,27 +1002,32 @@
   <dimension ref="A1:AM31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane xSplit="3420" topLeftCell="D1"/>
-      <selection activeCell="D12" sqref="A12:XFD12"/>
-      <selection pane="topRight" activeCell="AG2" sqref="AG1:AG1048576"/>
+      <pane xSplit="3400" topLeftCell="G1" activePane="topRight"/>
+      <selection activeCell="D14" sqref="A14:XFD14"/>
+      <selection pane="topRight" activeCell="AC22" sqref="AC22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="88" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="72" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
     <col min="10" max="15" width="0" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
-    <col min="21" max="25" width="0" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" customWidth="1"/>
+    <col min="19" max="19" width="0" hidden="1" customWidth="1"/>
+    <col min="21" max="25" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="12" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="48.1640625" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="20" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="0" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="10.83203125" customWidth="1"/>
     <col min="35" max="35" width="22.83203125" hidden="1" customWidth="1"/>
     <col min="36" max="37" width="0" hidden="1" customWidth="1"/>
   </cols>
@@ -1152,18 +1081,18 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
       <c r="AA1" t="s">
         <v>16</v>
       </c>
@@ -1179,10 +1108,10 @@
       <c r="AE1" t="s">
         <v>20</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AG1" s="2"/>
+      <c r="AG1" s="4"/>
       <c r="AH1" t="s">
         <v>21</v>
       </c>
@@ -1246,7 +1175,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" hidden="1">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1292,7 +1221,7 @@
       <c r="O3" t="s">
         <v>37</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="3">
         <v>168</v>
       </c>
       <c r="Q3" s="1" t="s">
@@ -1340,13 +1269,13 @@
       <c r="AE3" t="s">
         <v>41</v>
       </c>
-      <c r="AF3" s="3">
+      <c r="AF3" s="2">
         <v>16</v>
       </c>
-      <c r="AG3" s="3">
+      <c r="AG3" s="2">
         <v>2</v>
       </c>
-      <c r="AH3" s="3">
+      <c r="AH3" s="2">
         <v>192</v>
       </c>
       <c r="AI3" t="s">
@@ -1365,7 +1294,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" hidden="1">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1411,7 +1340,7 @@
       <c r="O4" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="3">
         <v>168</v>
       </c>
       <c r="Q4" s="1" t="s">
@@ -1453,13 +1382,13 @@
       <c r="AE4" t="s">
         <v>41</v>
       </c>
-      <c r="AF4" s="3">
+      <c r="AF4" s="2">
         <v>16</v>
       </c>
-      <c r="AG4" s="3">
+      <c r="AG4" s="2">
         <v>2</v>
       </c>
-      <c r="AH4" s="3">
+      <c r="AH4" s="2">
         <v>192</v>
       </c>
       <c r="AI4" t="s">
@@ -1524,7 +1453,7 @@
       <c r="O5" t="s">
         <v>37</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="3">
         <v>168</v>
       </c>
       <c r="Q5" s="1" t="s">
@@ -1572,13 +1501,13 @@
       <c r="AE5" t="s">
         <v>41</v>
       </c>
-      <c r="AF5" s="3">
+      <c r="AF5" s="2">
         <v>24</v>
       </c>
-      <c r="AG5" s="3">
+      <c r="AG5" s="2">
         <v>2</v>
       </c>
-      <c r="AH5" s="3">
+      <c r="AH5" s="2">
         <v>192</v>
       </c>
       <c r="AI5" t="s">
@@ -1597,7 +1526,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:39" hidden="1">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -1643,7 +1572,7 @@
       <c r="O6" t="s">
         <v>37</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="3">
         <v>168</v>
       </c>
       <c r="Q6" s="1" t="s">
@@ -1685,13 +1614,13 @@
       <c r="AE6" t="s">
         <v>41</v>
       </c>
-      <c r="AF6" s="3">
+      <c r="AF6" s="2">
         <v>16</v>
       </c>
-      <c r="AG6" s="3">
+      <c r="AG6" s="2">
         <v>2</v>
       </c>
-      <c r="AH6" s="3">
+      <c r="AH6" s="2">
         <v>192</v>
       </c>
       <c r="AI6" t="s">
@@ -1756,7 +1685,7 @@
       <c r="O7" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="3">
         <v>168</v>
       </c>
       <c r="Q7" s="1" t="s">
@@ -1804,13 +1733,13 @@
       <c r="AE7" t="s">
         <v>41</v>
       </c>
-      <c r="AF7" s="3">
+      <c r="AF7" s="2">
         <v>24</v>
       </c>
-      <c r="AG7" s="3">
+      <c r="AG7" s="2">
         <v>2</v>
       </c>
-      <c r="AH7" s="3">
+      <c r="AH7" s="2">
         <v>192</v>
       </c>
       <c r="AI7" t="s">
@@ -1829,7 +1758,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:39" hidden="1">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1875,7 +1804,7 @@
       <c r="O8" t="s">
         <v>37</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8" s="3">
         <v>168</v>
       </c>
       <c r="Q8" s="1" t="s">
@@ -1919,13 +1848,13 @@
       <c r="AE8" t="s">
         <v>41</v>
       </c>
-      <c r="AF8" s="3">
+      <c r="AF8" s="2">
         <v>16</v>
       </c>
-      <c r="AG8" s="3">
+      <c r="AG8" s="2">
         <v>2</v>
       </c>
-      <c r="AH8" s="3">
+      <c r="AH8" s="2">
         <v>192</v>
       </c>
       <c r="AI8" t="s">
@@ -1944,7 +1873,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:39" hidden="1">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1990,7 +1919,7 @@
       <c r="O9" t="s">
         <v>37</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="3">
         <v>168</v>
       </c>
       <c r="Q9" s="1" t="s">
@@ -2038,13 +1967,13 @@
       <c r="AE9" t="s">
         <v>41</v>
       </c>
-      <c r="AF9" s="3">
+      <c r="AF9" s="2">
         <v>16</v>
       </c>
-      <c r="AG9" s="3">
+      <c r="AG9" s="2">
         <v>2</v>
       </c>
-      <c r="AH9" s="3">
+      <c r="AH9" s="2">
         <v>192</v>
       </c>
       <c r="AI9" t="s">
@@ -2109,7 +2038,7 @@
       <c r="O10" t="s">
         <v>37</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10" s="3">
         <v>168</v>
       </c>
       <c r="Q10" s="1" t="s">
@@ -2153,13 +2082,13 @@
       <c r="AE10" t="s">
         <v>41</v>
       </c>
-      <c r="AF10" s="3">
+      <c r="AF10" s="2">
         <v>24</v>
       </c>
-      <c r="AG10" s="3">
+      <c r="AG10" s="2">
         <v>2</v>
       </c>
-      <c r="AH10" s="3">
+      <c r="AH10" s="2">
         <v>192</v>
       </c>
       <c r="AI10" t="s">
@@ -2224,7 +2153,7 @@
       <c r="O11" t="s">
         <v>37</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11" s="3">
         <v>168</v>
       </c>
       <c r="Q11" s="1" t="s">
@@ -2272,13 +2201,13 @@
       <c r="AE11" t="s">
         <v>41</v>
       </c>
-      <c r="AF11" s="3">
+      <c r="AF11" s="2">
         <v>24</v>
       </c>
-      <c r="AG11" s="3">
+      <c r="AG11" s="2">
         <v>2</v>
       </c>
-      <c r="AH11" s="3">
+      <c r="AH11" s="2">
         <v>192</v>
       </c>
       <c r="AI11" t="s">
@@ -2297,122 +2226,122 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
-      <c r="A12" t="s">
+    <row r="12" spans="1:39" s="5" customFormat="1">
+      <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="5">
         <v>20760</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
         <v>15.08</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
         <v>1</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12" s="6">
         <v>168</v>
       </c>
-      <c r="Q12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA12" t="s">
+      <c r="Q12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="R12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="U12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="V12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="W12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="X12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AB12">
+      <c r="AB12" s="5">
         <v>140</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AC12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AD12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AE12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AF12" s="3">
+      <c r="AF12" s="8">
         <v>24</v>
       </c>
-      <c r="AG12" s="3">
+      <c r="AG12" s="8">
         <v>2</v>
       </c>
-      <c r="AH12" s="3">
+      <c r="AH12" s="8">
         <v>192</v>
       </c>
-      <c r="AI12" t="s">
+      <c r="AI12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AJ12" t="s">
+      <c r="AJ12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AK12" t="s">
+      <c r="AK12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AL12" t="s">
+      <c r="AL12" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="AM12" t="s">
+      <c r="AM12" s="5" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2462,7 +2391,7 @@
       <c r="O13" t="s">
         <v>37</v>
       </c>
-      <c r="P13" s="4">
+      <c r="P13" s="3">
         <v>168</v>
       </c>
       <c r="Q13" s="1" t="s">
@@ -2510,13 +2439,13 @@
       <c r="AE13" t="s">
         <v>41</v>
       </c>
-      <c r="AF13" s="3">
+      <c r="AF13" s="2">
         <v>24</v>
       </c>
-      <c r="AG13" s="3">
+      <c r="AG13" s="2">
         <v>2</v>
       </c>
-      <c r="AH13" s="3">
+      <c r="AH13" s="2">
         <v>192</v>
       </c>
       <c r="AI13" t="s">
@@ -2535,122 +2464,122 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
-      <c r="A14" t="s">
+    <row r="14" spans="1:39" s="5" customFormat="1">
+      <c r="A14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="5">
         <v>511</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
         <v>15.75</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
+      <c r="J14" s="5">
+        <v>0</v>
+      </c>
+      <c r="K14" s="5">
         <v>1</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="P14" s="4">
+      <c r="P14" s="6">
         <v>168</v>
       </c>
-      <c r="Q14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="Z14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA14" t="s">
+      <c r="Q14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="U14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="V14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="W14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="X14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AB14">
+      <c r="AB14" s="5">
         <v>140</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AC14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AD14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AE14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AF14" s="3">
+      <c r="AF14" s="8">
         <v>24</v>
       </c>
-      <c r="AG14" s="3">
+      <c r="AG14" s="8">
         <v>2</v>
       </c>
-      <c r="AH14" s="3">
+      <c r="AH14" s="8">
         <v>192</v>
       </c>
-      <c r="AI14" t="s">
+      <c r="AI14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AJ14" t="s">
+      <c r="AJ14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AK14" t="s">
+      <c r="AK14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AL14" t="s">
+      <c r="AL14" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="AM14" t="s">
+      <c r="AM14" s="5" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2700,7 +2629,7 @@
       <c r="O15" t="s">
         <v>37</v>
       </c>
-      <c r="P15" s="4">
+      <c r="P15" s="3">
         <v>180</v>
       </c>
       <c r="Q15" s="1" t="s">
@@ -2744,13 +2673,13 @@
       <c r="AE15" t="s">
         <v>41</v>
       </c>
-      <c r="AF15" s="3">
+      <c r="AF15" s="2">
         <v>16</v>
       </c>
-      <c r="AG15" s="3">
+      <c r="AG15" s="2">
         <v>2</v>
       </c>
-      <c r="AH15" s="3">
+      <c r="AH15" s="2">
         <v>256</v>
       </c>
       <c r="AI15" t="s">
@@ -2815,7 +2744,7 @@
       <c r="O16" t="s">
         <v>37</v>
       </c>
-      <c r="P16" s="4">
+      <c r="P16" s="3">
         <v>180</v>
       </c>
       <c r="Q16" s="1" t="s">
@@ -2859,13 +2788,13 @@
       <c r="AE16" t="s">
         <v>41</v>
       </c>
-      <c r="AF16" s="3">
+      <c r="AF16" s="2">
         <v>16</v>
       </c>
-      <c r="AG16" s="3">
+      <c r="AG16" s="2">
         <v>2</v>
       </c>
-      <c r="AH16" s="3">
+      <c r="AH16" s="2">
         <v>256</v>
       </c>
       <c r="AI16" t="s">
@@ -2930,7 +2859,7 @@
       <c r="O17" t="s">
         <v>37</v>
       </c>
-      <c r="P17" s="4">
+      <c r="P17" s="3">
         <v>180</v>
       </c>
       <c r="Q17" s="1" t="s">
@@ -2974,13 +2903,13 @@
       <c r="AE17" t="s">
         <v>41</v>
       </c>
-      <c r="AF17" s="3">
+      <c r="AF17" s="2">
         <v>24</v>
       </c>
-      <c r="AG17" s="3">
+      <c r="AG17" s="2">
         <v>2</v>
       </c>
-      <c r="AH17" s="3">
+      <c r="AH17" s="2">
         <v>256</v>
       </c>
       <c r="AI17" t="s">
@@ -3045,7 +2974,7 @@
       <c r="O18" t="s">
         <v>37</v>
       </c>
-      <c r="P18" s="4">
+      <c r="P18" s="3">
         <v>180</v>
       </c>
       <c r="Q18" s="1" t="s">
@@ -3089,13 +3018,13 @@
       <c r="AE18" t="s">
         <v>41</v>
       </c>
-      <c r="AF18" s="3">
+      <c r="AF18" s="2">
         <v>24</v>
       </c>
-      <c r="AG18" s="3">
+      <c r="AG18" s="2">
         <v>2</v>
       </c>
-      <c r="AH18" s="3">
+      <c r="AH18" s="2">
         <v>256</v>
       </c>
       <c r="AI18" t="s">
@@ -3160,7 +3089,7 @@
       <c r="O19" t="s">
         <v>37</v>
       </c>
-      <c r="P19" s="4">
+      <c r="P19" s="3">
         <v>180</v>
       </c>
       <c r="Q19" s="1" t="s">
@@ -3204,13 +3133,13 @@
       <c r="AE19" t="s">
         <v>41</v>
       </c>
-      <c r="AF19" s="3">
+      <c r="AF19" s="2">
         <v>24</v>
       </c>
-      <c r="AG19" s="3">
+      <c r="AG19" s="2">
         <v>2</v>
       </c>
-      <c r="AH19" s="3">
+      <c r="AH19" s="2">
         <v>256</v>
       </c>
       <c r="AI19" t="s">
@@ -3275,7 +3204,7 @@
       <c r="O20" t="s">
         <v>37</v>
       </c>
-      <c r="P20" s="4">
+      <c r="P20" s="3">
         <v>180</v>
       </c>
       <c r="Q20" s="1" t="s">
@@ -3319,13 +3248,13 @@
       <c r="AE20" t="s">
         <v>41</v>
       </c>
-      <c r="AF20" s="3">
+      <c r="AF20" s="2">
         <v>24</v>
       </c>
-      <c r="AG20" s="3">
+      <c r="AG20" s="2">
         <v>2</v>
       </c>
-      <c r="AH20" s="3">
+      <c r="AH20" s="2">
         <v>256</v>
       </c>
       <c r="AI20" t="s">
@@ -3344,7 +3273,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:39" hidden="1">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -3390,7 +3319,7 @@
       <c r="O21" t="s">
         <v>37</v>
       </c>
-      <c r="P21" s="4">
+      <c r="P21" s="3">
         <v>168</v>
       </c>
       <c r="Q21" s="1" t="s">
@@ -3434,13 +3363,13 @@
       <c r="AE21" t="s">
         <v>41</v>
       </c>
-      <c r="AF21" s="3">
+      <c r="AF21" s="2">
         <v>16</v>
       </c>
-      <c r="AG21" s="3">
+      <c r="AG21" s="2">
         <v>2</v>
       </c>
-      <c r="AH21" s="3">
+      <c r="AH21" s="2">
         <v>192</v>
       </c>
       <c r="AI21" t="s">
@@ -3459,126 +3388,126 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:39">
-      <c r="A22" t="s">
+    <row r="22" spans="1:39" s="5" customFormat="1">
+      <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="5">
         <v>496</v>
       </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
         <v>12.72</v>
       </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
+      <c r="J22" s="5">
+        <v>0</v>
+      </c>
+      <c r="K22" s="5">
         <v>1</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="P22" s="4">
+      <c r="P22" s="6">
         <v>168</v>
       </c>
-      <c r="Q22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="W22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="X22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="Y22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="Z22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA22" t="s">
+      <c r="Q22" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="R22" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="S22" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="T22" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="U22" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="V22" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="W22" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="X22" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y22" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z22" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AB22">
+      <c r="AB22" s="5">
         <v>140</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="AC22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AD22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AE22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AF22" s="3">
+      <c r="AF22" s="8">
         <v>24</v>
       </c>
-      <c r="AG22" s="3">
+      <c r="AG22" s="8">
         <v>2</v>
       </c>
-      <c r="AH22" s="3">
+      <c r="AH22" s="8">
         <v>192</v>
       </c>
-      <c r="AI22" t="s">
+      <c r="AI22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AJ22" t="s">
+      <c r="AJ22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AK22" t="s">
+      <c r="AK22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AL22" t="s">
+      <c r="AL22" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="AM22" t="s">
+      <c r="AM22" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:39" hidden="1">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -3624,7 +3553,7 @@
       <c r="O23" t="s">
         <v>37</v>
       </c>
-      <c r="P23" s="4">
+      <c r="P23" s="3">
         <v>168</v>
       </c>
       <c r="Q23" s="1" t="s">
@@ -3672,13 +3601,13 @@
       <c r="AE23" t="s">
         <v>41</v>
       </c>
-      <c r="AF23" s="3">
+      <c r="AF23" s="2">
         <v>16</v>
       </c>
-      <c r="AG23" s="3">
+      <c r="AG23" s="2">
         <v>2</v>
       </c>
-      <c r="AH23" s="3">
+      <c r="AH23" s="2">
         <v>192</v>
       </c>
       <c r="AI23" t="s">
@@ -3743,7 +3672,7 @@
       <c r="O24" t="s">
         <v>37</v>
       </c>
-      <c r="P24" s="4">
+      <c r="P24" s="3">
         <v>168</v>
       </c>
       <c r="Q24" s="1" t="s">
@@ -3791,13 +3720,13 @@
       <c r="AE24" t="s">
         <v>41</v>
       </c>
-      <c r="AF24" s="3">
+      <c r="AF24" s="2">
         <v>24</v>
       </c>
-      <c r="AG24" s="3">
+      <c r="AG24" s="2">
         <v>2</v>
       </c>
-      <c r="AH24" s="3">
+      <c r="AH24" s="2">
         <v>192</v>
       </c>
       <c r="AI24" t="s">
@@ -3862,7 +3791,7 @@
       <c r="O25" t="s">
         <v>37</v>
       </c>
-      <c r="P25" s="4">
+      <c r="P25" s="3">
         <v>168</v>
       </c>
       <c r="Q25" s="1" t="s">
@@ -3910,13 +3839,13 @@
       <c r="AE25" t="s">
         <v>41</v>
       </c>
-      <c r="AF25" s="3">
+      <c r="AF25" s="2">
         <v>24</v>
       </c>
-      <c r="AG25" s="3">
+      <c r="AG25" s="2">
         <v>2</v>
       </c>
-      <c r="AH25" s="3">
+      <c r="AH25" s="2">
         <v>192</v>
       </c>
       <c r="AI25" t="s">
@@ -3935,7 +3864,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:39">
+    <row r="26" spans="1:39" hidden="1">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -3981,7 +3910,7 @@
       <c r="O26" t="s">
         <v>37</v>
       </c>
-      <c r="P26" s="4">
+      <c r="P26" s="3">
         <v>168</v>
       </c>
       <c r="Q26" s="1" t="s">
@@ -4029,13 +3958,13 @@
       <c r="AE26" t="s">
         <v>41</v>
       </c>
-      <c r="AF26" s="3">
+      <c r="AF26" s="2">
         <v>16</v>
       </c>
-      <c r="AG26" s="3">
+      <c r="AG26" s="2">
         <v>2</v>
       </c>
-      <c r="AH26" s="3">
+      <c r="AH26" s="2">
         <v>192</v>
       </c>
       <c r="AI26" t="s">
@@ -4100,7 +4029,7 @@
       <c r="O27" t="s">
         <v>37</v>
       </c>
-      <c r="P27" s="4">
+      <c r="P27" s="3">
         <v>168</v>
       </c>
       <c r="Q27" s="1" t="s">
@@ -4144,13 +4073,13 @@
       <c r="AE27" t="s">
         <v>41</v>
       </c>
-      <c r="AF27" s="3">
+      <c r="AF27" s="2">
         <v>24</v>
       </c>
-      <c r="AG27" s="3">
+      <c r="AG27" s="2">
         <v>2</v>
       </c>
-      <c r="AH27" s="3">
+      <c r="AH27" s="2">
         <v>192</v>
       </c>
       <c r="AI27" t="s">
@@ -4169,7 +4098,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:39">
+    <row r="28" spans="1:39" hidden="1">
       <c r="A28" t="s">
         <v>124</v>
       </c>
@@ -4215,7 +4144,7 @@
       <c r="O28" t="s">
         <v>37</v>
       </c>
-      <c r="P28" s="4">
+      <c r="P28" s="3">
         <v>168</v>
       </c>
       <c r="Q28" s="1" t="s">
@@ -4261,13 +4190,13 @@
       <c r="AE28" t="s">
         <v>41</v>
       </c>
-      <c r="AF28" s="3">
+      <c r="AF28" s="2">
         <v>16</v>
       </c>
-      <c r="AG28" s="3">
+      <c r="AG28" s="2">
         <v>2</v>
       </c>
-      <c r="AH28" s="3">
+      <c r="AH28" s="2">
         <v>256</v>
       </c>
       <c r="AI28" t="s">
@@ -4332,7 +4261,7 @@
       <c r="O29" t="s">
         <v>37</v>
       </c>
-      <c r="P29" s="4">
+      <c r="P29" s="3">
         <v>168</v>
       </c>
       <c r="Q29" s="1" t="s">
@@ -4380,13 +4309,13 @@
       <c r="AE29" t="s">
         <v>41</v>
       </c>
-      <c r="AF29" s="3">
+      <c r="AF29" s="2">
         <v>24</v>
       </c>
-      <c r="AG29" s="3">
+      <c r="AG29" s="2">
         <v>2</v>
       </c>
-      <c r="AH29" s="3">
+      <c r="AH29" s="2">
         <v>192</v>
       </c>
       <c r="AI29" t="s">
@@ -4451,7 +4380,7 @@
       <c r="O30" t="s">
         <v>37</v>
       </c>
-      <c r="P30" s="4">
+      <c r="P30" s="3">
         <v>168</v>
       </c>
       <c r="Q30" s="1" t="s">
@@ -4499,13 +4428,13 @@
       <c r="AE30" t="s">
         <v>41</v>
       </c>
-      <c r="AF30" s="3">
+      <c r="AF30" s="2">
         <v>24</v>
       </c>
-      <c r="AG30" s="3">
+      <c r="AG30" s="2">
         <v>2</v>
       </c>
-      <c r="AH30" s="3">
+      <c r="AH30" s="2">
         <v>192</v>
       </c>
       <c r="AI30" t="s">
@@ -4570,7 +4499,7 @@
       <c r="O31" t="s">
         <v>37</v>
       </c>
-      <c r="P31" s="4">
+      <c r="P31" s="3">
         <v>168</v>
       </c>
       <c r="Q31" s="1" t="s">
@@ -4618,13 +4547,13 @@
       <c r="AE31" t="s">
         <v>41</v>
       </c>
-      <c r="AF31" s="3">
+      <c r="AF31" s="2">
         <v>24</v>
       </c>
-      <c r="AG31" s="3">
+      <c r="AG31" s="2">
         <v>2</v>
       </c>
-      <c r="AH31" s="3">
+      <c r="AH31" s="2">
         <v>192</v>
       </c>
       <c r="AI31" t="s">
@@ -4649,7 +4578,7 @@
     <mergeCell ref="AF1:AG1"/>
   </mergeCells>
   <conditionalFormatting sqref="AB1:AB1048576">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4659,12 +4588,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="13" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4676,7 +4605,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W36">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4688,7 +4617,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I31">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4700,7 +4629,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G31">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4712,6 +4641,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3:AF31">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH3:AH31">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P31">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -4723,32 +4676,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH31">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P31">
+  <conditionalFormatting sqref="I5:I31">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added a decision matrix on page2 of STM32matrix.xlsx
</commit_message>
<xml_diff>
--- a/STM32matrix.xlsx
+++ b/STM32matrix.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2820" yWindow="20" windowWidth="13140" windowHeight="14920" tabRatio="1000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="156">
   <si>
     <t>Datasheets</t>
   </si>
@@ -472,6 +473,21 @@
   </si>
   <si>
     <t>MHz</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -526,7 +542,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -572,8 +588,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -582,9 +610,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -593,8 +618,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -617,6 +646,12 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -639,29 +674,15 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1002,8 +1023,8 @@
   <dimension ref="A1:AM31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane xSplit="3400" topLeftCell="G1" activePane="topRight"/>
-      <selection activeCell="D14" sqref="A14:XFD14"/>
+      <pane xSplit="4480" topLeftCell="R1" activePane="topRight"/>
+      <selection activeCell="D13" sqref="A13:XFD13"/>
       <selection pane="topRight" activeCell="AC22" sqref="AC22"/>
     </sheetView>
   </sheetViews>
@@ -1081,18 +1102,18 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
       <c r="AA1" t="s">
         <v>16</v>
       </c>
@@ -1108,10 +1129,10 @@
       <c r="AE1" t="s">
         <v>20</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AG1" s="4"/>
+      <c r="AG1" s="8"/>
       <c r="AH1" t="s">
         <v>21</v>
       </c>
@@ -1175,7 +1196,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:39" hidden="1">
+    <row r="3" spans="1:39">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1294,7 +1315,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:39" hidden="1">
+    <row r="4" spans="1:39">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1526,7 +1547,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:39" hidden="1">
+    <row r="6" spans="1:39">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -1758,7 +1779,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:39" hidden="1">
+    <row r="8" spans="1:39">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1873,7 +1894,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:39" hidden="1">
+    <row r="9" spans="1:39">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -2226,126 +2247,126 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:39" s="5" customFormat="1">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:39" s="4" customFormat="1">
+      <c r="A12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>20760</v>
       </c>
-      <c r="H12" s="5">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5">
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
         <v>15.08</v>
       </c>
-      <c r="J12" s="5">
-        <v>0</v>
-      </c>
-      <c r="K12" s="5">
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
         <v>1</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="M12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="O12" s="5" t="s">
+      <c r="O12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="5">
         <v>168</v>
       </c>
-      <c r="Q12" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="R12" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="S12" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="T12" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="U12" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="V12" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="W12" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="X12" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="Y12" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="Z12" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA12" s="5" t="s">
+      <c r="Q12" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="U12" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="V12" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="W12" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="X12" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y12" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z12" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AB12" s="5">
+      <c r="AB12" s="4">
         <v>140</v>
       </c>
-      <c r="AC12" s="5" t="s">
+      <c r="AC12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AD12" s="5" t="s">
+      <c r="AD12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AE12" s="5" t="s">
+      <c r="AE12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AF12" s="8">
+      <c r="AF12" s="7">
         <v>24</v>
       </c>
-      <c r="AG12" s="8">
+      <c r="AG12" s="7">
         <v>2</v>
       </c>
-      <c r="AH12" s="8">
+      <c r="AH12" s="7">
         <v>192</v>
       </c>
-      <c r="AI12" s="5" t="s">
+      <c r="AI12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AJ12" s="5" t="s">
+      <c r="AJ12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AK12" s="5" t="s">
+      <c r="AK12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AL12" s="5" t="s">
+      <c r="AL12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AM12" s="5" t="s">
+      <c r="AM12" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:39" hidden="1">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -2464,122 +2485,122 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:39" s="5" customFormat="1">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:39" s="4" customFormat="1">
+      <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>511</v>
       </c>
-      <c r="H14" s="5">
-        <v>0</v>
-      </c>
-      <c r="I14" s="5">
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
         <v>15.75</v>
       </c>
-      <c r="J14" s="5">
-        <v>0</v>
-      </c>
-      <c r="K14" s="5">
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
         <v>1</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="M14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="N14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="O14" s="5" t="s">
+      <c r="O14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="P14" s="6">
+      <c r="P14" s="5">
         <v>168</v>
       </c>
-      <c r="Q14" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="R14" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="S14" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="T14" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="U14" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="V14" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="W14" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="X14" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="Y14" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="Z14" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA14" s="5" t="s">
+      <c r="Q14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="T14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="U14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="V14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="W14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="X14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AB14" s="5">
+      <c r="AB14" s="4">
         <v>140</v>
       </c>
-      <c r="AC14" s="5" t="s">
+      <c r="AC14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AD14" s="5" t="s">
+      <c r="AD14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AE14" s="5" t="s">
+      <c r="AE14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AF14" s="8">
+      <c r="AF14" s="7">
         <v>24</v>
       </c>
-      <c r="AG14" s="8">
+      <c r="AG14" s="7">
         <v>2</v>
       </c>
-      <c r="AH14" s="8">
+      <c r="AH14" s="7">
         <v>192</v>
       </c>
-      <c r="AI14" s="5" t="s">
+      <c r="AI14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AJ14" s="5" t="s">
+      <c r="AJ14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AK14" s="5" t="s">
+      <c r="AK14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AL14" s="5" t="s">
+      <c r="AL14" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="AM14" s="5" t="s">
+      <c r="AM14" s="4" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3388,126 +3409,126 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:39" s="5" customFormat="1">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:39" s="4" customFormat="1">
+      <c r="A22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <v>496</v>
       </c>
-      <c r="H22" s="5">
-        <v>0</v>
-      </c>
-      <c r="I22" s="5">
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
         <v>12.72</v>
       </c>
-      <c r="J22" s="5">
-        <v>0</v>
-      </c>
-      <c r="K22" s="5">
+      <c r="J22" s="4">
+        <v>0</v>
+      </c>
+      <c r="K22" s="4">
         <v>1</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="L22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="M22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="O22" s="5" t="s">
+      <c r="O22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="P22" s="6">
+      <c r="P22" s="5">
         <v>168</v>
       </c>
-      <c r="Q22" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="R22" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="S22" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="T22" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="U22" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="V22" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="W22" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="X22" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="Y22" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="Z22" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA22" s="5" t="s">
+      <c r="Q22" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="T22" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="U22" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="V22" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="W22" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="X22" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y22" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z22" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AB22" s="5">
+      <c r="AB22" s="4">
         <v>140</v>
       </c>
-      <c r="AC22" s="5" t="s">
+      <c r="AC22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AD22" s="5" t="s">
+      <c r="AD22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AE22" s="5" t="s">
+      <c r="AE22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AF22" s="8">
+      <c r="AF22" s="7">
         <v>24</v>
       </c>
-      <c r="AG22" s="8">
+      <c r="AG22" s="7">
         <v>2</v>
       </c>
-      <c r="AH22" s="8">
+      <c r="AH22" s="7">
         <v>192</v>
       </c>
-      <c r="AI22" s="5" t="s">
+      <c r="AI22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AJ22" s="5" t="s">
+      <c r="AJ22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AK22" s="5" t="s">
+      <c r="AK22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AL22" s="5" t="s">
+      <c r="AL22" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="AM22" s="5" t="s">
+      <c r="AM22" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:39" hidden="1">
+    <row r="23" spans="1:39">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -3864,7 +3885,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:39" hidden="1">
+    <row r="26" spans="1:39">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -4098,7 +4119,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:39" hidden="1">
+    <row r="28" spans="1:39">
       <c r="A28" t="s">
         <v>124</v>
       </c>
@@ -4588,7 +4609,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="13" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4689,6 +4710,126 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C6:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:9">
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" t="s">
+        <v>153</v>
+      </c>
+      <c r="I6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9">
+      <c r="C7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f>SUM(D7:H7)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9">
+      <c r="C8" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <f>SUM(D8:H8)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9">
+      <c r="C9" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <f>SUM(D9:H9)</f>
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>